<commit_message>
Pushed 20.03 Meeting Minutes, Made Minor Changes to Updated Hours Spreadsheet
</commit_message>
<xml_diff>
--- a/Admin/Group 16 Updated Hours (as of the end of Sprint 7).xlsx
+++ b/Admin/Group 16 Updated Hours (as of the end of Sprint 7).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fraser\Documents\GitHub\mgp-team16\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE4FE95C-5088-487F-ABAA-5069CA6BA3CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87200C61-D858-4E88-8C0D-2E3F7FB3E55C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38670" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Team Member</t>
   </si>
@@ -122,13 +122,16 @@
   </si>
   <si>
     <t>(Level 5 Managers Only)</t>
+  </si>
+  <si>
+    <t>(Pulled Directly from Meeting Minutes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -154,6 +157,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -175,12 +185,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,15 +511,14 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="48.7109375" bestFit="1" customWidth="1"/>
@@ -654,6 +664,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>29</v>
       </c>

</xml_diff>